<commit_message>
Fixed pertubation test sheets and updated LSETest.m
</commit_message>
<xml_diff>
--- a/test_files/compress_missing_data_test/pre-existing_sheet-compress-missing-data-sheet.xlsx
+++ b/test_files/compress_missing_data_test/pre-existing_sheet-compress-missing-data-sheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="443" yWindow="0" windowWidth="24398" windowHeight="15120" tabRatio="644" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="443" yWindow="0" windowWidth="24398" windowHeight="15120" tabRatio="644" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="13" r:id="rId1"/>
@@ -182,7 +182,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -191,6 +191,12 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -827,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection sqref="A1:M5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5859375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1088,7 +1094,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="A1:M5"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.703125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1097,208 +1103,208 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="6">
+      <c r="B1" s="9">
         <v>0.4</v>
       </c>
-      <c r="C1" s="6">
+      <c r="C1" s="9">
         <v>0.4</v>
       </c>
-      <c r="D1" s="6">
+      <c r="D1" s="9">
         <v>0.4</v>
       </c>
-      <c r="E1" s="6">
+      <c r="E1" s="9">
         <v>0.8</v>
       </c>
-      <c r="F1" s="6">
+      <c r="F1" s="9">
         <v>0.8</v>
       </c>
-      <c r="G1" s="6">
+      <c r="G1" s="9">
         <v>0.8</v>
       </c>
-      <c r="H1" s="6">
+      <c r="H1" s="9">
         <v>1.2</v>
       </c>
-      <c r="I1" s="6">
+      <c r="I1" s="9">
         <v>1.2</v>
       </c>
-      <c r="J1" s="6">
+      <c r="J1" s="9">
         <v>1.2</v>
       </c>
-      <c r="K1" s="6">
+      <c r="K1" s="9">
         <v>1.6</v>
       </c>
-      <c r="L1" s="6">
+      <c r="L1" s="9">
         <v>1.6</v>
       </c>
-      <c r="M1" s="6">
+      <c r="M1" s="9">
         <v>1.6</v>
       </c>
       <c r="N1" s="5"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="9">
         <v>111</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="9">
         <v>112</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="9">
         <v>113</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="9">
         <v>211</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="9">
         <v>212</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="9">
         <v>213</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="9">
         <v>311</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="9">
         <v>312</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="9">
         <v>313</v>
       </c>
-      <c r="K2" s="6">
+      <c r="K2" s="9">
         <v>411</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L2" s="9">
         <v>412</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M2" s="9">
         <v>413</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="9">
         <v>121</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="9">
         <v>122</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="9">
         <v>123</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="9">
         <v>221</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="9">
         <v>222</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="9">
         <v>223</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="9">
         <v>321</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="9">
         <v>322</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="9">
         <v>323</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="9">
         <v>421</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="9">
         <v>422</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="9">
         <v>423</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="6">
-        <v>0</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0</v>
-      </c>
-      <c r="G4" s="6">
-        <v>0</v>
-      </c>
-      <c r="H4" s="6">
-        <v>0</v>
-      </c>
-      <c r="I4" s="6">
-        <v>0</v>
-      </c>
-      <c r="J4" s="6">
-        <v>0</v>
-      </c>
-      <c r="K4" s="6">
-        <v>0</v>
-      </c>
-      <c r="L4" s="6">
-        <v>0</v>
-      </c>
-      <c r="M4" s="6">
+      <c r="A4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0</v>
+      </c>
+      <c r="G4" s="9">
+        <v>0</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0</v>
+      </c>
+      <c r="J4" s="9">
+        <v>0</v>
+      </c>
+      <c r="K4" s="9">
+        <v>0</v>
+      </c>
+      <c r="L4" s="9">
+        <v>0</v>
+      </c>
+      <c r="M4" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="6">
+      <c r="A5" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="9">
         <v>141</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="9">
         <v>142</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="9">
         <v>143</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="9">
         <v>241</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="9">
         <v>242</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="9">
         <v>243</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="9">
         <v>341</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="9">
         <v>342</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="9">
         <v>343</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="9">
         <v>441</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="9">
         <v>442</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="9">
         <v>443</v>
       </c>
     </row>

</xml_diff>